<commit_message>
Added PCB version 2.0.
Co-Authored-By: Artur Silva <artursilva0@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/PCB/harp behavior_BOM.xlsx
+++ b/PCB/harp behavior_BOM.xlsx
@@ -1,25 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\CR hw platform\1556 harp behavior\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_behavior\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859E56FD-CABB-4C5E-A2A2-A32C4A66B58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11610" yWindow="-15" windowWidth="11445" windowHeight="9645"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="207">
   <si>
     <t>Description</t>
   </si>
@@ -54,9 +68,6 @@
     <t>PCB</t>
   </si>
   <si>
-    <t>Assembly</t>
-  </si>
-  <si>
     <t>Components</t>
   </si>
   <si>
@@ -159,15 +170,6 @@
     <t>798-UX60-MB-5S8</t>
   </si>
   <si>
-    <t>USB Cable</t>
-  </si>
-  <si>
-    <t>USB A - MINI-B 0.8M - MINI-B 0.8M BLACK</t>
-  </si>
-  <si>
-    <t>538-88732-8502</t>
-  </si>
-  <si>
     <t>SMT 3.5 STEREO REEL</t>
   </si>
   <si>
@@ -180,9 +182,6 @@
     <t>606-7513D2-L</t>
   </si>
   <si>
-    <t>Tubos de Luz LED CML LIGHTPIPE</t>
-  </si>
-  <si>
     <t>649-67996-206HLF</t>
   </si>
   <si>
@@ -195,9 +194,6 @@
     <t>Licensed under the TAPR Open Hardware License (www.tapr.org/OHL)</t>
   </si>
   <si>
-    <t>Copyright 2017 Artur Silva and Filipe Carvalho</t>
-  </si>
-  <si>
     <t>652-CR0402FX-1004GLF</t>
   </si>
   <si>
@@ -240,15 +236,6 @@
     <t>RES SMD 330Ω OHM 1% 0402</t>
   </si>
   <si>
-    <t>2h</t>
-  </si>
-  <si>
-    <t>83.5mmx83.5mm 5x</t>
-  </si>
-  <si>
-    <t>Acrylic</t>
-  </si>
-  <si>
     <t>Conectores modulares/Conectores de Ethernet 8/8 R/A MOD JACK</t>
   </si>
   <si>
@@ -333,9 +320,6 @@
     <t>20.1550M/4-E -  Pluggable Terminal Block, 3.5 mm, 4 Ways</t>
   </si>
   <si>
-    <t>20.1550M/2-E  Pluggable Terminal Block, 3.5 mm, 2 Ways</t>
-  </si>
-  <si>
     <t>20.1550M/3-E -  Pluggable Terminal Block, 3.5 mm, 3 Ways</t>
   </si>
   <si>
@@ -417,12 +401,6 @@
     <t>FERRITE BEAD 600Ω 500mA 300mΩ 0805</t>
   </si>
   <si>
-    <t>667-ERJ-2RKF1602X</t>
-  </si>
-  <si>
-    <t>RES SMD 16kΩ 1% 0402</t>
-  </si>
-  <si>
     <t>667-ERJ-2RKF2402X</t>
   </si>
   <si>
@@ -459,21 +437,12 @@
     <t>IC8, IC11</t>
   </si>
   <si>
-    <t>IC10</t>
-  </si>
-  <si>
     <t>IC6, IC13, IC15, IC17</t>
   </si>
   <si>
-    <t>IC12, IC14, IC16</t>
-  </si>
-  <si>
     <t>C6, C7</t>
   </si>
   <si>
-    <t>C41, C42</t>
-  </si>
-  <si>
     <t>C29, C32</t>
   </si>
   <si>
@@ -495,18 +464,6 @@
     <t>R23, R24, R25, R26, R29, R30, R31, R32</t>
   </si>
   <si>
-    <t>R16, R18, R21, R22, R27, R28, R33, R34, R35, R36, R37, R38</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>R10, R17, R39, R40, R41, R42, R43, R44</t>
-  </si>
-  <si>
     <t>L2</t>
   </si>
   <si>
@@ -522,9 +479,6 @@
     <t>X1, X2</t>
   </si>
   <si>
-    <t>X4, X5</t>
-  </si>
-  <si>
     <t>X3</t>
   </si>
   <si>
@@ -591,9 +545,6 @@
     <t>RES SMD 95.3kΩ 1% 0402</t>
   </si>
   <si>
-    <t>F1</t>
-  </si>
-  <si>
     <t>81-GRM155R61E105MA2D</t>
   </si>
   <si>
@@ -603,9 +554,6 @@
     <t>C37, C43</t>
   </si>
   <si>
-    <t>C5, C11, C13, C15, C19, C20, C21, C22, C23, C24, C25, C26, C27, C28, C30, C31, C35, C37, C39, C40, C43, C44, C45, C46, C47, C48, C49</t>
-  </si>
-  <si>
     <t>R11, R20</t>
   </si>
   <si>
@@ -624,18 +572,6 @@
     <t>R12, R19</t>
   </si>
   <si>
-    <t>Ethernet Cable, Patch Lead, Cat5e, RJ45 Plug to RJ45 Plug, Beige, 500 mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WALL ADAPTER </t>
-  </si>
-  <si>
-    <t>AC/DC Power Supply, Class II, Fixed, 1 Output, 90 V, 264 V, 12 W, 12 V</t>
-  </si>
-  <si>
-    <t>VEL12US120-EU-JA</t>
-  </si>
-  <si>
     <t>D1, D2, D3, D4</t>
   </si>
   <si>
@@ -654,25 +590,76 @@
     <t>R7, R11, R20</t>
   </si>
   <si>
-    <t>0603SFS100F/32-2 -  Fuse, Surface Mount, 0603SFS Series, 1 A, 32 VDC, Slow Blow, 0603</t>
-  </si>
-  <si>
     <t>584-AD8651ARZ</t>
   </si>
   <si>
     <t>Amplificadores de precisão 50MHz Low Distort Low Noise CMOS Prec</t>
   </si>
   <si>
-    <t>Internal</t>
-  </si>
-  <si>
-    <t>External</t>
+    <t>IC10, IC18</t>
+  </si>
+  <si>
+    <t>IC12, IC14, IC16, IC19</t>
+  </si>
+  <si>
+    <t>R13, R50</t>
+  </si>
+  <si>
+    <t>R14, R51</t>
+  </si>
+  <si>
+    <t>RES SMD 15kΩ 1% 0402</t>
+  </si>
+  <si>
+    <t>R16, R18, R21, R22, R27, R28, R33, R34, R35, R36, R37, R38, R48, R49</t>
+  </si>
+  <si>
+    <t>R10, R17, R39, R40, R41, R42, R43, R44, R52</t>
+  </si>
+  <si>
+    <t>C5, C11, C13, C15, C19, C20, C21, C22, C23, C24, C25, C26, C27, C28, C30, C31, C35, C37, C39, C40, C43, C44, C45, C46, C47, C48, C49, C52, C53</t>
+  </si>
+  <si>
+    <t>C41, C42, C50, C51</t>
+  </si>
+  <si>
+    <t>667-ERJ-2RKF1502X</t>
+  </si>
+  <si>
+    <t>X5</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>Copyright 2021 Artur Silva and Filipe Carvalho</t>
+  </si>
+  <si>
+    <t>Horizontal, Header, 3.5 mm, 5 Ways, 10 A, 250 V, Through Hole Right Angle</t>
+  </si>
+  <si>
+    <t>20.155MH/5-E</t>
+  </si>
+  <si>
+    <t>20.1550M/5-E -  Pluggable Terminal Block, 3.5 mm, 5 Ways</t>
+  </si>
+  <si>
+    <t>83.5mmx83.5mm</t>
+  </si>
+  <si>
+    <t>LED CML LIGHTPIPE</t>
+  </si>
+  <si>
+    <t>VER12US120-JA - AC/DC Power Supply, Class II, Fixed, 1 Output, 90 V, 264 V, 12 W, 12 V</t>
+  </si>
+  <si>
+    <t>20.1550M/2-E  - Pluggable Terminal Block, 3.5 mm, 2 Ways</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -1187,27 +1174,27 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1220,32 +1207,15 @@
     <xf numFmtId="164" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1380,6 +1350,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1415,6 +1402,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1590,20 +1594,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J83"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K80" sqref="K80"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="92.140625" style="1" bestFit="1" customWidth="1"/>
@@ -1618,8 +1622,8 @@
     <col min="13" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -1644,1772 +1648,1685 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>56</v>
+    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="C2" s="8">
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="G2" s="21">
+        <v>12</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="16">
         <v>0.56100000000000005</v>
       </c>
-      <c r="H2" s="21">
+      <c r="H2" s="16">
         <f t="shared" ref="H2:H4" si="0">G2*C2</f>
         <v>0.56100000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
-        <v>78</v>
+    <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="C3" s="8">
         <v>0</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="G3" s="21">
+        <v>12</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="16">
         <v>3.96</v>
       </c>
-      <c r="H3" s="21">
+      <c r="H3" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
-        <v>78</v>
+    <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="C4" s="8">
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="G4" s="21">
+        <v>12</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="16">
         <v>3.37</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="16">
         <f t="shared" si="0"/>
         <v>3.37</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
-        <v>143</v>
+    <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="C5" s="8">
         <v>2</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="21">
+        <v>12</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="16">
         <v>0.52800000000000002</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="16">
         <f t="shared" ref="H5:H11" si="1">G5*C5</f>
         <v>1.056</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="20" t="s">
-        <v>62</v>
+    <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="C6" s="8">
         <v>1</v>
       </c>
       <c r="D6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="21">
+      <c r="G6" s="16">
         <v>4.24</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="16">
         <f t="shared" si="1"/>
         <v>4.24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="20" t="s">
-        <v>81</v>
+    <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>72</v>
       </c>
       <c r="C7" s="8">
         <v>1</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="G7" s="21">
+        <v>130</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="16">
         <v>3.26</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="16">
         <f>G7*C7</f>
         <v>3.26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="20" t="s">
-        <v>147</v>
+    <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>134</v>
       </c>
       <c r="C8" s="8">
         <v>4</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="21">
+        <v>12</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="16">
         <v>0.33900000000000002</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="16">
         <f>G8*C8</f>
         <v>1.3560000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="20" t="s">
-        <v>144</v>
+    <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>132</v>
       </c>
       <c r="C9" s="8">
         <v>1</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="21">
+        <v>12</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="16">
         <v>5.32</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="16">
         <f t="shared" si="1"/>
         <v>5.32</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="20" t="s">
-        <v>145</v>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>133</v>
       </c>
       <c r="C10" s="8">
         <v>2</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>213</v>
+        <v>186</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="G10" s="21">
+        <v>12</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G10" s="16">
         <v>2.5299999999999998</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="16">
         <f t="shared" si="1"/>
         <v>5.0599999999999996</v>
       </c>
-      <c r="I10" s="18"/>
-    </row>
-    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
-        <v>146</v>
+    </row>
+    <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
+        <v>187</v>
       </c>
       <c r="C11" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="G11" s="21">
+        <v>12</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="16">
         <v>1.46</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="16">
         <f t="shared" si="1"/>
-        <v>1.46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
-        <v>148</v>
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>188</v>
       </c>
       <c r="C12" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="21">
+        <v>12</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="16">
         <v>0.73599999999999999</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="16">
         <f t="shared" ref="H12:H20" si="2">G12*C12</f>
-        <v>2.2080000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
-        <v>84</v>
+        <v>2.944</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="C13" s="8">
         <v>2</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="G13" s="21">
+        <v>12</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="16">
         <v>0.28899999999999998</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="16">
         <f t="shared" si="2"/>
         <v>0.57799999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="20" t="s">
-        <v>87</v>
+    <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
+        <v>78</v>
       </c>
       <c r="C14" s="8">
         <v>2</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="G14" s="21">
+        <v>12</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G14" s="16">
         <v>0.70599999999999996</v>
       </c>
-      <c r="H14" s="21">
+      <c r="H14" s="16">
         <f t="shared" si="2"/>
         <v>1.4119999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
-        <v>89</v>
+    <row r="15" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="C15" s="8">
         <v>4</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G15" s="21">
+        <v>12</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="16">
         <v>0.69699999999999995</v>
       </c>
-      <c r="H15" s="21">
+      <c r="H15" s="16">
         <f t="shared" si="2"/>
         <v>2.7879999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
-        <v>90</v>
+    <row r="16" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="C16" s="8">
         <v>4</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="G16" s="21">
+        <v>12</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="16">
         <v>0.23799999999999999</v>
       </c>
-      <c r="H16" s="21">
+      <c r="H16" s="16">
         <f t="shared" si="2"/>
         <v>0.95199999999999996</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="20" t="s">
-        <v>93</v>
+      <c r="B17" s="15" t="s">
+        <v>84</v>
       </c>
       <c r="C17" s="8">
         <v>3</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="21">
+        <v>12</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" s="16">
         <v>0.29799999999999999</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="16">
         <f t="shared" si="2"/>
         <v>0.89399999999999991</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="s">
-        <v>115</v>
+      <c r="B18" s="15" t="s">
+        <v>105</v>
       </c>
       <c r="C18" s="8">
         <v>3</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="G18" s="21">
+        <v>12</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="16">
         <v>0.48499999999999999</v>
       </c>
-      <c r="H18" s="21">
+      <c r="H18" s="16">
         <f t="shared" si="2"/>
         <v>1.4550000000000001</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="20" t="s">
-        <v>205</v>
+      <c r="B19" s="15" t="s">
+        <v>179</v>
       </c>
       <c r="C19" s="8">
         <v>4</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="G19" s="21">
+        <v>12</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" s="16">
         <v>0.38300000000000001</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="16">
         <f t="shared" si="2"/>
         <v>1.532</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
-        <v>183</v>
+      <c r="B20" s="15" t="s">
+        <v>163</v>
       </c>
       <c r="C20" s="8">
         <v>1</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="G20" s="21">
+        <v>12</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G20" s="16">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="H20" s="21">
+      <c r="H20" s="16">
         <f t="shared" si="2"/>
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
-        <v>149</v>
+      <c r="B21" s="15" t="s">
+        <v>135</v>
       </c>
       <c r="C21" s="8">
         <v>2</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" s="21">
+        <v>12</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="16">
         <v>9.4E-2</v>
       </c>
-      <c r="H21" s="21">
+      <c r="H21" s="16">
         <f t="shared" ref="H21:H23" si="3">G21*C21</f>
         <v>0.188</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
-        <v>32</v>
+      <c r="B22" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="C22" s="8">
         <v>1</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="21">
+        <v>12</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="16">
         <v>9.4E-2</v>
       </c>
-      <c r="H22" s="21">
+      <c r="H22" s="16">
         <f t="shared" si="3"/>
         <v>9.4E-2</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="20" t="s">
-        <v>150</v>
+      <c r="B23" s="15" t="s">
+        <v>195</v>
       </c>
       <c r="C23" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="G23" s="21">
+        <v>12</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="16">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="H23" s="21">
+      <c r="H23" s="16">
         <f t="shared" si="3"/>
-        <v>0.17</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="15" t="s">
         <v>194</v>
       </c>
       <c r="C24" s="8">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21">
-        <f t="shared" ref="H24:H55" si="4">G24*C24</f>
+        <v>7</v>
+      </c>
+      <c r="F24" s="9">
+        <v>2310530</v>
+      </c>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16">
+        <f t="shared" ref="H24:H54" si="4">G24*C24</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="20" t="s">
-        <v>151</v>
+      <c r="B25" s="15" t="s">
+        <v>136</v>
       </c>
       <c r="C25" s="8">
         <v>2</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="21">
+        <v>12</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="16">
         <v>0.104</v>
       </c>
-      <c r="H25" s="21">
+      <c r="H25" s="16">
         <f t="shared" si="4"/>
         <v>0.20799999999999999</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="20" t="s">
-        <v>193</v>
+      <c r="B26" s="15" t="s">
+        <v>172</v>
       </c>
       <c r="C26" s="8">
         <v>0</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="E26" s="8"/>
-      <c r="F26" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="G26" s="21">
+      <c r="F26" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G26" s="16">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="H26" s="21">
+      <c r="H26" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="20" t="s">
-        <v>152</v>
+      <c r="B27" s="15" t="s">
+        <v>137</v>
       </c>
       <c r="C27" s="8">
         <v>1</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="21">
+        <v>12</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="16">
         <v>0.311</v>
       </c>
-      <c r="H27" s="21">
+      <c r="H27" s="16">
         <f t="shared" si="4"/>
         <v>0.311</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="20" t="s">
-        <v>181</v>
+      <c r="B28" s="15" t="s">
+        <v>161</v>
       </c>
       <c r="C28" s="8">
         <v>6</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G28" s="21">
+        <v>12</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="16">
         <v>0.189</v>
       </c>
-      <c r="H28" s="21">
+      <c r="H28" s="16">
         <f t="shared" si="4"/>
         <v>1.1339999999999999</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="20" t="s">
-        <v>153</v>
+      <c r="B29" s="15" t="s">
+        <v>138</v>
       </c>
       <c r="C29" s="8">
         <v>1</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="G29" s="21">
+        <v>12</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G29" s="16">
         <v>1.85</v>
       </c>
-      <c r="H29" s="21">
+      <c r="H29" s="16">
         <f t="shared" si="4"/>
         <v>1.85</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="20" t="s">
-        <v>180</v>
+      <c r="B30" s="15" t="s">
+        <v>160</v>
       </c>
       <c r="C30" s="8">
         <v>2</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="G30" s="21">
+        <v>12</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G30" s="16">
         <v>0.83299999999999996</v>
       </c>
-      <c r="H30" s="21">
+      <c r="H30" s="16">
         <f t="shared" si="4"/>
         <v>1.6659999999999999</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="20" t="s">
-        <v>171</v>
+      <c r="B31" s="15" t="s">
+        <v>151</v>
       </c>
       <c r="C31" s="8">
         <v>2</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="G31" s="21">
+        <v>12</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G31" s="16">
         <v>0.75700000000000001</v>
       </c>
-      <c r="H31" s="21">
+      <c r="H31" s="16">
         <f t="shared" si="4"/>
         <v>1.514</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="20" t="s">
-        <v>175</v>
+      <c r="B32" s="15" t="s">
+        <v>155</v>
       </c>
       <c r="C32" s="8">
         <v>1</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="G32" s="21">
+        <v>12</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="G32" s="16">
         <v>0.51</v>
       </c>
-      <c r="H32" s="21">
+      <c r="H32" s="16">
         <f t="shared" si="4"/>
         <v>0.51</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="20" t="s">
-        <v>154</v>
+      <c r="B33" s="15" t="s">
+        <v>139</v>
       </c>
       <c r="C33" s="8">
         <v>3</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="G33" s="21">
+        <v>12</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G33" s="16">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="H33" s="21">
+      <c r="H33" s="16">
         <f t="shared" si="4"/>
         <v>0.255</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="20" t="s">
-        <v>94</v>
+      <c r="B34" s="15" t="s">
+        <v>85</v>
       </c>
       <c r="C34" s="8">
         <v>4</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="G34" s="21">
+        <v>12</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G34" s="16">
         <v>0.34899999999999998</v>
       </c>
-      <c r="H34" s="21">
+      <c r="H34" s="16">
         <f t="shared" si="4"/>
         <v>1.3959999999999999</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="20" t="s">
-        <v>195</v>
+      <c r="B35" s="15" t="s">
+        <v>173</v>
       </c>
       <c r="C35" s="8">
         <v>0</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="G35" s="21">
+        <v>12</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="G35" s="16">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="H35" s="21">
+      <c r="H35" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="20" t="s">
-        <v>200</v>
+      <c r="B36" s="15" t="s">
+        <v>178</v>
       </c>
       <c r="C36" s="8">
         <v>0</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="G36" s="21">
+        <v>12</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G36" s="16">
         <v>0.247</v>
       </c>
-      <c r="H36" s="21">
+      <c r="H36" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="20" t="s">
-        <v>155</v>
+      <c r="B37" s="15" t="s">
+        <v>140</v>
       </c>
       <c r="C37" s="8">
         <v>1</v>
       </c>
       <c r="D37" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="G37" s="21">
+      <c r="G37" s="16">
         <v>9.4E-2</v>
       </c>
-      <c r="H37" s="21">
+      <c r="H37" s="16">
         <f t="shared" si="4"/>
         <v>9.4E-2</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="20" t="s">
-        <v>210</v>
+      <c r="B38" s="15" t="s">
+        <v>184</v>
       </c>
       <c r="C38" s="8">
         <v>3</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="G38" s="21">
+        <v>12</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G38" s="16">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="H38" s="21">
+      <c r="H38" s="16">
         <f t="shared" si="4"/>
         <v>0.255</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="20" t="s">
-        <v>200</v>
+      <c r="B39" s="15" t="s">
+        <v>178</v>
       </c>
       <c r="C39" s="8">
         <v>2</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="G39" s="21">
+        <v>12</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G39" s="16">
         <v>0.20399999999999999</v>
       </c>
-      <c r="H39" s="21">
+      <c r="H39" s="16">
         <f t="shared" si="4"/>
         <v>0.40799999999999997</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
-        <v>173</v>
+      <c r="B40" s="15" t="s">
+        <v>153</v>
       </c>
       <c r="C40" s="8">
         <v>1</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="G40" s="21">
+        <v>12</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G40" s="16">
         <v>0.128</v>
       </c>
-      <c r="H40" s="21">
+      <c r="H40" s="16">
         <f t="shared" si="4"/>
         <v>0.128</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="20" t="s">
-        <v>156</v>
+      <c r="B41" s="15" t="s">
+        <v>141</v>
       </c>
       <c r="C41" s="8">
         <v>3</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="G41" s="21">
+        <v>12</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G41" s="16">
         <v>0.187</v>
       </c>
-      <c r="H41" s="21">
+      <c r="H41" s="16">
         <f t="shared" si="4"/>
         <v>0.56099999999999994</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B42" s="20" t="s">
-        <v>158</v>
+    <row r="42" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B42" s="15" t="s">
+        <v>192</v>
       </c>
       <c r="C42" s="8">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F42" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21">
+        <v>16</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="20" t="s">
-        <v>157</v>
+      <c r="B43" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="C43" s="8">
         <v>8</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="G43" s="21">
+        <v>12</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="G43" s="16">
         <v>0.23799999999999999</v>
       </c>
-      <c r="H43" s="21">
+      <c r="H43" s="16">
         <f t="shared" si="4"/>
         <v>1.9039999999999999</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="20" t="s">
-        <v>159</v>
+      <c r="B44" s="15" t="s">
+        <v>190</v>
       </c>
       <c r="C44" s="8">
+        <v>2</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="G44" s="16">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="H44" s="16">
+        <f t="shared" si="4"/>
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="C45" s="8">
+        <v>2</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="G45" s="16">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="H45" s="16">
+        <f t="shared" si="4"/>
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46" s="8">
         <v>1</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="G44" s="21">
+      <c r="D46" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="G46" s="16">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="H44" s="21">
+      <c r="H46" s="16">
         <f t="shared" si="4"/>
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="C45" s="8">
-        <v>1</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="G45" s="21">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="H45" s="21">
-        <f t="shared" si="4"/>
-        <v>8.5000000000000006E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="C46" s="8">
-        <v>1</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F46" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="G46" s="21">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="H46" s="21">
-        <f t="shared" si="4"/>
-        <v>8.5000000000000006E-2</v>
-      </c>
-    </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="20" t="s">
-        <v>187</v>
+      <c r="B47" s="15" t="s">
+        <v>167</v>
       </c>
       <c r="C47" s="8">
         <v>1</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F47" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="G47" s="21">
+        <v>12</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="G47" s="16">
         <v>0.128</v>
       </c>
-      <c r="H47" s="21">
+      <c r="H47" s="16">
         <f t="shared" si="4"/>
         <v>0.128</v>
       </c>
     </row>
     <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="20" t="s">
-        <v>161</v>
+      <c r="B48" s="15" t="s">
+        <v>193</v>
       </c>
       <c r="C48" s="8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F48" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21">
+        <v>16</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="20" t="s">
-        <v>39</v>
+      <c r="B49" s="15" t="s">
+        <v>38</v>
       </c>
       <c r="C49" s="8">
         <v>1</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="G49" s="21">
+        <v>12</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G49" s="16">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="H49" s="21">
+      <c r="H49" s="16">
         <f t="shared" si="4"/>
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="20" t="s">
-        <v>190</v>
+      <c r="B50" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="C50" s="8">
         <v>1</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>211</v>
+        <v>55</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F50" s="16">
-        <v>1843816</v>
-      </c>
-      <c r="G50" s="21">
-        <v>0.71399999999999997</v>
-      </c>
-      <c r="H50" s="21">
+        <v>12</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G50" s="16">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="H50" s="16">
         <f t="shared" si="4"/>
-        <v>0.71399999999999997</v>
+        <v>0.57499999999999996</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="20" t="s">
-        <v>51</v>
+      <c r="B51" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="C51" s="8">
         <v>1</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F51" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="G51" s="21">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="H51" s="21">
+        <v>12</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G51" s="16">
+        <v>1.75</v>
+      </c>
+      <c r="H51" s="16">
         <f t="shared" si="4"/>
-        <v>0.57499999999999996</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="20" t="s">
-        <v>14</v>
+      <c r="B52" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="C52" s="8">
         <v>1</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F52" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" s="21">
-        <v>1.75</v>
-      </c>
-      <c r="H52" s="21">
+        <v>12</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G52" s="16">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="H52" s="16">
         <f t="shared" si="4"/>
-        <v>1.75</v>
+        <v>0.71499999999999997</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="20" t="s">
-        <v>68</v>
+      <c r="B53" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="C53" s="8">
         <v>1</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F53" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="G53" s="21">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="H53" s="21">
+        <v>12</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="G53" s="16">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="H53" s="16">
         <f t="shared" si="4"/>
-        <v>0.71499999999999997</v>
+        <v>1.1100000000000001</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="20" t="s">
-        <v>24</v>
+      <c r="B54" s="15" t="s">
+        <v>143</v>
       </c>
       <c r="C54" s="8">
         <v>1</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>165</v>
+        <v>39</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F54" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="G54" s="21">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="H54" s="21">
-        <f t="shared" si="4"/>
-        <v>1.1100000000000001</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="C55" s="8">
-        <v>1</v>
-      </c>
-      <c r="D55" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E55" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F55" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G55" s="21">
+      <c r="G54" s="16">
         <v>9.4E-2</v>
       </c>
-      <c r="H55" s="21">
+      <c r="H54" s="16">
         <f t="shared" si="4"/>
         <v>9.4E-2</v>
       </c>
     </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="8">
+        <v>2</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G55" s="16">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="H55" s="16">
+        <f t="shared" ref="H55:H56" si="5">G55*C55</f>
+        <v>0.17</v>
+      </c>
+    </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="20" t="s">
-        <v>163</v>
+      <c r="B56" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="C56" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>131</v>
+        <v>50</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F56" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="G56" s="21">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="H56" s="21">
-        <f t="shared" ref="H56:H57" si="5">G56*C56</f>
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C57" s="8">
-        <v>1</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E57" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F57" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="G57" s="21">
+        <v>12</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G56" s="16">
         <v>0.377</v>
       </c>
-      <c r="H57" s="21">
+      <c r="H56" s="16">
         <f t="shared" si="5"/>
         <v>0.377</v>
       </c>
     </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="8">
+        <v>3</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G57" s="16">
+        <v>1.27</v>
+      </c>
+      <c r="H57" s="16">
+        <f t="shared" ref="H57" si="6">G57*C57</f>
+        <v>3.81</v>
+      </c>
+    </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="9" t="s">
-        <v>126</v>
+      <c r="B58" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="C58" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F58" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="G58" s="24">
-        <v>1.27</v>
-      </c>
-      <c r="H58" s="24">
-        <f t="shared" ref="H58:H59" si="6">G58*C58</f>
-        <v>3.81</v>
+        <v>12</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G58" s="16">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="H58" s="16">
+        <f t="shared" ref="H58:H61" si="7">G58*C58</f>
+        <v>0.83899999999999997</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="9"/>
+      <c r="B59" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="C59" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>201</v>
+        <v>118</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F59" s="23">
-        <v>1526101</v>
-      </c>
-      <c r="G59" s="24">
-        <v>1.43</v>
-      </c>
-      <c r="H59" s="24">
-        <f t="shared" si="6"/>
-        <v>4.29</v>
+        <v>12</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G59" s="16">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H59" s="16">
+        <f t="shared" si="7"/>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="20" t="s">
-        <v>43</v>
+      <c r="B60" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="C60" s="8">
         <v>1</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F60" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G60" s="21">
-        <v>0.83899999999999997</v>
-      </c>
-      <c r="H60" s="21">
-        <f t="shared" ref="H60:H69" si="7">G60*C60</f>
-        <v>0.83899999999999997</v>
+        <v>7</v>
+      </c>
+      <c r="F60" s="9">
+        <v>1360143</v>
+      </c>
+      <c r="G60" s="16">
+        <v>0.184</v>
+      </c>
+      <c r="H60" s="16">
+        <f t="shared" si="7"/>
+        <v>0.184</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="20" t="s">
-        <v>46</v>
+      <c r="B61" s="15" t="s">
+        <v>147</v>
       </c>
       <c r="C61" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F61" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G61" s="21">
-        <v>2.52</v>
-      </c>
-      <c r="H61" s="21">
+        <v>7</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G61" s="16">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="H61" s="16">
         <f t="shared" si="7"/>
-        <v>2.52</v>
+        <v>0.33600000000000002</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="15" t="s">
+        <v>148</v>
+      </c>
       <c r="C62" s="8">
         <v>1</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F62" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G62" s="21">
-        <v>0.68799999999999994</v>
-      </c>
-      <c r="H62" s="21">
-        <f t="shared" si="7"/>
-        <v>0.68799999999999994</v>
+        <v>7</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G62" s="16">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="H62" s="16">
+        <f>G62*C62</f>
+        <v>0.43099999999999999</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="18" t="s">
-        <v>127</v>
+      <c r="B63" s="15" t="s">
+        <v>198</v>
       </c>
       <c r="C63" s="8">
         <v>1</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>128</v>
+        <v>200</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F63" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="G63" s="24">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="H63" s="21">
-        <f t="shared" si="7"/>
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="20" t="s">
-        <v>202</v>
+        <v>7</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="G63" s="16">
+        <v>0.92</v>
+      </c>
+      <c r="H63" s="16">
+        <f>G63*C63</f>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="C64" s="8">
         <v>1</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>203</v>
+        <v>93</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F64" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="G64" s="21">
-        <v>10.57</v>
-      </c>
-      <c r="H64" s="21">
-        <f t="shared" si="7"/>
-        <v>10.57</v>
-      </c>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="C65" s="8">
-        <v>1</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F65" s="16">
-        <v>1360143</v>
-      </c>
-      <c r="G65" s="21">
-        <v>0.184</v>
-      </c>
-      <c r="H65" s="21">
-        <f t="shared" si="7"/>
-        <v>0.184</v>
-      </c>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" s="20"/>
-      <c r="C66" s="8">
-        <v>2</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E66" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F66" s="16">
-        <v>2575215</v>
-      </c>
-      <c r="G66" s="21">
-        <v>0.245</v>
-      </c>
-      <c r="H66" s="21">
-        <f t="shared" si="7"/>
-        <v>0.49</v>
-      </c>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" s="20"/>
-      <c r="C67" s="8">
-        <v>2</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F67" s="16">
-        <v>2575216</v>
-      </c>
-      <c r="G67" s="21">
-        <v>0.375</v>
-      </c>
-      <c r="H67" s="21">
-        <f t="shared" si="7"/>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" s="20"/>
+      <c r="F64" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G64" s="16">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="H64" s="16">
+        <f>G64*C64</f>
+        <v>0.67400000000000004</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="10">
+        <f>SUM(C2:C64)</f>
+        <v>167</v>
+      </c>
+      <c r="D65" s="5"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="12"/>
+      <c r="D66" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="E66" s="12"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="13">
+        <f>88.48/5</f>
+        <v>17.696000000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I67" s="14"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C68" s="8">
         <v>1</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>103</v>
+        <v>205</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F68" s="16">
-        <v>2575217</v>
-      </c>
-      <c r="G68" s="21">
-        <v>0.49099999999999999</v>
-      </c>
-      <c r="H68" s="21">
-        <f t="shared" si="7"/>
-        <v>0.49099999999999999</v>
-      </c>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B69" s="20" t="s">
-        <v>166</v>
-      </c>
+      <c r="F68" s="9">
+        <v>2524430</v>
+      </c>
+      <c r="G68" s="16">
+        <v>14.35</v>
+      </c>
+      <c r="H68" s="16">
+        <f>G68*C68</f>
+        <v>14.35</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C69" s="8">
         <v>2</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>70</v>
+        <v>206</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F69" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="G69" s="21">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="H69" s="21">
-        <f t="shared" si="7"/>
-        <v>0.33600000000000002</v>
-      </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B70" s="20" t="s">
-        <v>167</v>
-      </c>
+      <c r="F69" s="9">
+        <v>2575215</v>
+      </c>
+      <c r="G69" s="16">
+        <v>0.245</v>
+      </c>
+      <c r="H69" s="16">
+        <f>G69*C69</f>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C70" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F70" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="G70" s="21">
-        <v>0.43099999999999999</v>
-      </c>
-      <c r="H70" s="21">
+      <c r="F70" s="9">
+        <v>2575216</v>
+      </c>
+      <c r="G70" s="16">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="H70" s="16">
         <f>G70*C70</f>
-        <v>0.86199999999999999</v>
-      </c>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B71" s="20" t="s">
-        <v>168</v>
-      </c>
+        <v>0.71899999999999997</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C71" s="8">
         <v>1</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>102</v>
+        <v>202</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F71" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="G71" s="21">
-        <v>0.67400000000000004</v>
-      </c>
-      <c r="H71" s="21">
+      <c r="F71" s="9">
+        <v>2575218</v>
+      </c>
+      <c r="G71" s="16">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="H71" s="16">
         <f>G71*C71</f>
-        <v>0.67400000000000004</v>
-      </c>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B72" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C72" s="10">
-        <f>SUM(C2:C71)</f>
-        <v>168</v>
-      </c>
-      <c r="D72" s="5"/>
-      <c r="E72" s="10"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="7">
-        <f>SUM(H2:H71)</f>
-        <v>83.840000000000018</v>
-      </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B73" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C73" s="12"/>
-      <c r="D73" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="E73" s="12"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="13">
-        <f>88.48/5</f>
-        <v>17.696000000000002</v>
-      </c>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B74" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C74" s="12"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="12"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B75" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C75" s="12"/>
-      <c r="D75" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E75" s="12"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="13">
-        <f>2*8.5</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G76" s="15" t="s">
+        <v>0.98499999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C72" s="8">
+        <v>1</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F72" s="9">
+        <v>2575217</v>
+      </c>
+      <c r="G72" s="16">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="H72" s="16">
+        <f t="shared" ref="H72" si="8">G72*C72</f>
+        <v>0.95899999999999996</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C73" s="8">
+        <v>1</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G73" s="16">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="H73" s="16">
+        <f>G73*C73</f>
+        <v>0.68799999999999994</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G76" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H76" s="14">
-        <f>SUM(H72:H75)</f>
-        <v>123.53600000000002</v>
-      </c>
-      <c r="I76" s="19">
-        <v>125</v>
-      </c>
-      <c r="J76" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H77" s="19"/>
-      <c r="I77" s="19">
-        <f>ROUND(H76*1.3,0)+50</f>
-        <v>211</v>
-      </c>
-      <c r="J77" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H78" s="19"/>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>57</v>
-      </c>
-      <c r="H79" s="19"/>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B80" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C83" s="1"/>
-      <c r="E83" s="1"/>
+      <c r="H76" s="18">
+        <f>SUM(H2:H73)</f>
+        <v>102.239</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>